<commit_message>
add notes for Windows users
</commit_message>
<xml_diff>
--- a/crypto.xlsx
+++ b/crypto.xlsx
@@ -28,16 +28,16 @@
     <t xml:space="preserve">Book Value</t>
   </si>
   <si>
-    <t xml:space="preserve">Dogecoin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cat Token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Squirrel Finance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meme</t>
+    <t xml:space="preserve">Bitcoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethereum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Litecoin</t>
   </si>
 </sst>
 </file>
@@ -149,44 +149,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,128 +207,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="29.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="22.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="29.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="5" t="n">
         <v>44245.8125</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>1500</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="C2" s="7" t="n">
         <v>3500.1505</v>
       </c>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="7" t="n">
         <v>6500.3507</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="7" t="n">
         <v>0.7105</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>0.7105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>